<commit_message>
refactor: updated to only generate a single json pool config incl. relationships and messages
</commit_message>
<xml_diff>
--- a/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance/tools/snapshot-creator-v2/Config/PerformanceTestData.xlsx
+++ b/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance/tools/snapshot-creator-v2/Config/PerformanceTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance\tools\snapshot-creator-v2\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance.SnapshotCreator.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EB3797-D92E-4CF0-B683-4B25E1261B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D0D313-A305-4EB2-8B1E-6676F9B7FEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="-165" windowWidth="29400" windowHeight="13080" tabRatio="235" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
+    <workbookView xWindow="405" yWindow="2730" windowWidth="35550" windowHeight="11010" tabRatio="318" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="heavy" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CA4C26A-54D3-D4EA-B670-CD1E0CFC7FC2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A77805-3055-1268-ABDF-7997506269F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -427,22 +427,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>11205</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1393717</xdr:colOff>
+      <xdr:colOff>1382512</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>136460</xdr:rowOff>
+      <xdr:rowOff>114048</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20EF7462-60EB-A0B4-076F-92AFAF242242}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEF05A9D-A168-B2C4-F504-F34C057C4C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -458,7 +458,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="593911" y="1938618"/>
+          <a:off x="582706" y="1916206"/>
           <a:ext cx="6828571" cy="2019048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -482,16 +482,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>873375</xdr:colOff>
+      <xdr:colOff>878248</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>114048</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87E2F651-58A3-A8CD-20EE-16E30D74C702}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{918CD441-B3A0-2710-D16D-22D95B6B7D08}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -507,7 +507,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="679174" y="1913283"/>
+          <a:off x="672353" y="1916206"/>
           <a:ext cx="6828571" cy="2019048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -841,7 +841,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,7 @@
       </c>
       <c r="Q2" s="9">
         <f>na1_*ma1_+na2_*ma2_+na3_*ma3_</f>
-        <v>780000</v>
+        <v>775000</v>
       </c>
       <c r="R2" s="9">
         <f>na1_*I3+na2_*I4+na3_*I5</f>
@@ -1007,11 +1007,11 @@
       </c>
       <c r="V2" s="9">
         <f>nc1_*I6+nc2_*I7+nc3_*I8</f>
-        <v>780000</v>
+        <v>774990</v>
       </c>
       <c r="W2" s="10">
         <f>Q2-V2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X2" s="9">
         <f>nc1_*rc_1+nc2_*rc_2+nc3_*rc_3</f>
@@ -1039,8 +1039,7 @@
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11">
-        <f>10+K3</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I3" s="22">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na1_)*M3)+L3</f>
@@ -1253,7 +1252,7 @@
       </c>
       <c r="I7" s="22">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc2_)*M7)+L7</f>
-        <v>9750</v>
+        <v>9687</v>
       </c>
       <c r="J7" s="16" t="str">
         <f t="shared" si="0"/>
@@ -1307,7 +1306,7 @@
       </c>
       <c r="I8" s="22">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc3_)*M8)+L8</f>
-        <v>19500</v>
+        <v>19375</v>
       </c>
       <c r="J8" s="16" t="str">
         <f t="shared" si="0"/>
@@ -1373,7 +1372,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2:L8"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1394,7 @@
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.140625" customWidth="1"/>
+    <col min="18" max="18" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -1908,7 +1907,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2:L8"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1928,7 @@
     <col min="14" max="14" width="34" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.7109375" customWidth="1"/>
     <col min="18" max="18" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="42" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="33.5703125" bestFit="1" customWidth="1"/>
@@ -1970,10 +1969,10 @@
       <c r="J1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -2315,6 +2314,7 @@
         <v>0.24</v>
       </c>
       <c r="H7" s="11">
+        <f>8+K7</f>
         <v>8</v>
       </c>
       <c r="I7" s="22">

</xml_diff>